<commit_message>
wave data updated with new group of sprites
git-svn-id: https://svn.code.sf.net/p/castle-defender/code/trunk@46 44b1cee5-f01f-473f-a638-7a13f5ae6cd1
</commit_message>
<xml_diff>
--- a/waves/waves and enemies.xlsx
+++ b/waves/waves and enemies.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="79">
   <si>
     <t>wave</t>
   </si>
@@ -208,6 +208,60 @@
   </si>
   <si>
     <t>variants</t>
+  </si>
+  <si>
+    <t>cut("E1","exp1");</t>
+  </si>
+  <si>
+    <t>cut("E2","exp2");</t>
+  </si>
+  <si>
+    <t>cut("E3","exp3");</t>
+  </si>
+  <si>
+    <t>cut("E4","exp4");</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -533,10 +587,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH21"/>
+  <dimension ref="A1:AN24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF11" sqref="AF11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,9 +607,14 @@
     <col min="24" max="26" width="2.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="3" bestFit="1" customWidth="1"/>
     <col min="28" max="30" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="4.5703125" customWidth="1"/>
+    <col min="37" max="37" width="4" customWidth="1"/>
+    <col min="38" max="38" width="3.85546875" customWidth="1"/>
+    <col min="39" max="39" width="3.7109375" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -623,7 +682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -728,12 +787,31 @@
       <c r="AG2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AH2" t="str">
-        <f>INDEX(AA2:AD11,1,1)</f>
-        <v>1a</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AH2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ2" t="str">
+        <f>VLOOKUP(AA2,$AH$6:$AI$24,2,FALSE)</f>
+        <v>a</v>
+      </c>
+      <c r="AK2" t="str">
+        <f t="shared" ref="AK2:AM2" si="2">VLOOKUP(AB2,$AH$6:$AI$24,2,FALSE)</f>
+        <v>c</v>
+      </c>
+      <c r="AL2" t="str">
+        <f t="shared" si="2"/>
+        <v>d</v>
+      </c>
+      <c r="AM2" t="str">
+        <f t="shared" si="2"/>
+        <v>e</v>
+      </c>
+      <c r="AN2" t="str">
+        <f>CONCATENATE(AJ2,AK2,AL2,AM2)</f>
+        <v>acde</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -801,7 +879,7 @@
         <v>45</v>
       </c>
       <c r="W3" t="str">
-        <f t="shared" ref="W3:W20" si="2">VLOOKUP(G3,$AF$2:$AG$6,2,FALSE)</f>
+        <f t="shared" ref="W3:W20" si="3">VLOOKUP(G3,$AF$2:$AG$6,2,FALSE)</f>
         <v>a</v>
       </c>
       <c r="X3" t="str">
@@ -817,19 +895,19 @@
         <v>b</v>
       </c>
       <c r="AA3" t="str">
-        <f t="shared" ref="AA3:AA21" si="3">CONCATENATE(C3,W3)</f>
+        <f t="shared" ref="AA3:AA21" si="4">CONCATENATE(C3,W3)</f>
         <v>1a</v>
       </c>
       <c r="AB3" t="str">
-        <f t="shared" ref="AB3:AB21" si="4">CONCATENATE(D3,X3)</f>
+        <f t="shared" ref="AB3:AB21" si="5">CONCATENATE(D3,X3)</f>
         <v>1c</v>
       </c>
       <c r="AC3" t="str">
-        <f t="shared" ref="AC3:AC21" si="5">CONCATENATE(E3,Y3)</f>
+        <f t="shared" ref="AC3:AC21" si="6">CONCATENATE(E3,Y3)</f>
         <v>2a</v>
       </c>
       <c r="AD3" t="str">
-        <f t="shared" ref="AD3:AD21" si="6">CONCATENATE(F3,Z3)</f>
+        <f t="shared" ref="AD3:AD21" si="7">CONCATENATE(F3,Z3)</f>
         <v>2b</v>
       </c>
       <c r="AF3" s="1" t="s">
@@ -838,8 +916,31 @@
       <c r="AG3" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="AH3" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ3" t="str">
+        <f t="shared" ref="AJ3:AJ21" si="8">VLOOKUP(AA3,$AH$6:$AI$24,2,FALSE)</f>
+        <v>a</v>
+      </c>
+      <c r="AK3" t="str">
+        <f t="shared" ref="AK3:AK21" si="9">VLOOKUP(AB3,$AH$6:$AI$24,2,FALSE)</f>
+        <v>c</v>
+      </c>
+      <c r="AL3" t="str">
+        <f t="shared" ref="AL3:AL21" si="10">VLOOKUP(AC3,$AH$6:$AI$24,2,FALSE)</f>
+        <v>d</v>
+      </c>
+      <c r="AM3" t="str">
+        <f t="shared" ref="AM3:AM21" si="11">VLOOKUP(AD3,$AH$6:$AI$24,2,FALSE)</f>
+        <v>e</v>
+      </c>
+      <c r="AN3" t="str">
+        <f t="shared" ref="AN3:AN21" si="12">CONCATENATE(AJ3,AK3,AL3,AM3)</f>
+        <v>acde</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -907,7 +1008,7 @@
         <v>55</v>
       </c>
       <c r="W4" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>a</v>
       </c>
       <c r="X4" t="str">
@@ -923,1378 +1024,1864 @@
         <v>a</v>
       </c>
       <c r="AA4" t="str">
+        <f t="shared" si="4"/>
+        <v>5a</v>
+      </c>
+      <c r="AB4" t="str">
+        <f t="shared" si="5"/>
+        <v>5c</v>
+      </c>
+      <c r="AC4" t="str">
+        <f t="shared" si="6"/>
+        <v>1a</v>
+      </c>
+      <c r="AD4" t="str">
+        <f t="shared" si="7"/>
+        <v>2a</v>
+      </c>
+      <c r="AF4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AG4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ4" t="str">
+        <f t="shared" si="8"/>
+        <v>m</v>
+      </c>
+      <c r="AK4" t="str">
+        <f t="shared" si="9"/>
+        <v>n</v>
+      </c>
+      <c r="AL4" t="str">
+        <f t="shared" si="10"/>
+        <v>a</v>
+      </c>
+      <c r="AM4" t="str">
+        <f t="shared" si="11"/>
+        <v>d</v>
+      </c>
+      <c r="AN4" t="str">
+        <f t="shared" si="12"/>
+        <v>mnad</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>10</v>
+      </c>
+      <c r="M5">
+        <v>15</v>
+      </c>
+      <c r="N5">
+        <v>25</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>10</v>
+      </c>
+      <c r="S5">
+        <v>45</v>
+      </c>
+      <c r="T5">
+        <v>55</v>
+      </c>
+      <c r="U5">
+        <v>65</v>
+      </c>
+      <c r="V5">
+        <v>25</v>
+      </c>
+      <c r="W5" t="str">
         <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X5" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y5" t="str">
+        <f t="shared" si="0"/>
+        <v>b</v>
+      </c>
+      <c r="Z5" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA5" t="str">
+        <f t="shared" si="4"/>
         <v>5a</v>
       </c>
-      <c r="AB4" t="str">
+      <c r="AB5" t="str">
+        <f t="shared" si="5"/>
+        <v>1a</v>
+      </c>
+      <c r="AC5" t="str">
+        <f t="shared" si="6"/>
+        <v>2b</v>
+      </c>
+      <c r="AD5" t="str">
+        <f t="shared" si="7"/>
+        <v>3a</v>
+      </c>
+      <c r="AF5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ5" t="str">
+        <f t="shared" si="8"/>
+        <v>m</v>
+      </c>
+      <c r="AK5" t="str">
+        <f t="shared" si="9"/>
+        <v>a</v>
+      </c>
+      <c r="AL5" t="str">
+        <f t="shared" si="10"/>
+        <v>e</v>
+      </c>
+      <c r="AM5" t="str">
+        <f t="shared" si="11"/>
+        <v>g</v>
+      </c>
+      <c r="AN5" t="str">
+        <f t="shared" si="12"/>
+        <v>maeg</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6">
+        <v>15</v>
+      </c>
+      <c r="L6">
+        <v>20</v>
+      </c>
+      <c r="M6">
+        <v>28</v>
+      </c>
+      <c r="N6">
+        <v>33</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>15</v>
+      </c>
+      <c r="R6">
+        <v>20</v>
+      </c>
+      <c r="S6">
+        <v>65</v>
+      </c>
+      <c r="T6">
+        <v>75</v>
+      </c>
+      <c r="U6">
+        <v>40</v>
+      </c>
+      <c r="V6">
+        <v>50</v>
+      </c>
+      <c r="W6" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X6" t="str">
+        <f t="shared" si="0"/>
+        <v>b</v>
+      </c>
+      <c r="Y6" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z6" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="AA6" t="str">
+        <f t="shared" si="4"/>
+        <v>1a</v>
+      </c>
+      <c r="AB6" t="str">
+        <f t="shared" si="5"/>
+        <v>2b</v>
+      </c>
+      <c r="AC6" t="str">
+        <f t="shared" si="6"/>
+        <v>3a</v>
+      </c>
+      <c r="AD6" t="str">
+        <f t="shared" si="7"/>
+        <v>3c</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AG6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>28</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ6" t="str">
+        <f t="shared" si="8"/>
+        <v>a</v>
+      </c>
+      <c r="AK6" t="str">
+        <f t="shared" si="9"/>
+        <v>e</v>
+      </c>
+      <c r="AL6" t="str">
+        <f t="shared" si="10"/>
+        <v>g</v>
+      </c>
+      <c r="AM6" t="str">
+        <f t="shared" si="11"/>
+        <v>h</v>
+      </c>
+      <c r="AN6" t="str">
+        <f t="shared" si="12"/>
+        <v>aegh</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7">
+        <v>11</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <v>25</v>
+      </c>
+      <c r="N7">
+        <v>30</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>7</v>
+      </c>
+      <c r="Q7">
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <v>23</v>
+      </c>
+      <c r="S7">
+        <v>15</v>
+      </c>
+      <c r="T7">
+        <v>23</v>
+      </c>
+      <c r="U7">
+        <v>10</v>
+      </c>
+      <c r="V7">
+        <v>20</v>
+      </c>
+      <c r="W7" t="str">
+        <f t="shared" si="3"/>
+        <v>c</v>
+      </c>
+      <c r="X7" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Y7" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Z7" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA7" t="str">
         <f t="shared" si="4"/>
         <v>5c</v>
       </c>
-      <c r="AC4" t="str">
+      <c r="AB7" t="str">
         <f t="shared" si="5"/>
-        <v>1a</v>
-      </c>
-      <c r="AD4" t="str">
+        <v>2c</v>
+      </c>
+      <c r="AC7" t="str">
         <f t="shared" si="6"/>
-        <v>2a</v>
-      </c>
-      <c r="AF4" s="1" t="s">
+        <v>3c</v>
+      </c>
+      <c r="AD7" t="str">
+        <f t="shared" si="7"/>
+        <v>6a</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>26</v>
+      </c>
+      <c r="AJ7" t="str">
+        <f t="shared" si="8"/>
+        <v>n</v>
+      </c>
+      <c r="AK7" t="str">
+        <f t="shared" si="9"/>
+        <v>f</v>
+      </c>
+      <c r="AL7" t="str">
+        <f t="shared" si="10"/>
+        <v>h</v>
+      </c>
+      <c r="AM7" t="str">
+        <f t="shared" si="11"/>
+        <v>o</v>
+      </c>
+      <c r="AN7" t="str">
+        <f t="shared" si="12"/>
+        <v>nfho</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>6</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" t="s">
         <v>11</v>
       </c>
-      <c r="AG4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5">
-        <v>3</v>
-      </c>
-      <c r="L5">
-        <v>10</v>
-      </c>
-      <c r="M5">
+      <c r="L8">
         <v>15</v>
       </c>
-      <c r="N5">
+      <c r="M8">
+        <v>30</v>
+      </c>
+      <c r="N8">
+        <v>50</v>
+      </c>
+      <c r="O8">
+        <v>11</v>
+      </c>
+      <c r="P8">
+        <v>16</v>
+      </c>
+      <c r="Q8">
+        <v>22</v>
+      </c>
+      <c r="R8">
+        <v>30</v>
+      </c>
+      <c r="S8">
+        <v>15</v>
+      </c>
+      <c r="T8">
+        <v>20</v>
+      </c>
+      <c r="U8">
         <v>25</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>10</v>
-      </c>
-      <c r="S5">
+      <c r="V8">
         <v>45</v>
       </c>
-      <c r="T5">
-        <v>55</v>
-      </c>
-      <c r="U5">
-        <v>65</v>
-      </c>
-      <c r="V5">
-        <v>25</v>
-      </c>
-      <c r="W5" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X5" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y5" t="str">
-        <f t="shared" si="0"/>
-        <v>b</v>
-      </c>
-      <c r="Z5" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA5" t="str">
+      <c r="W8" t="str">
         <f t="shared" si="3"/>
-        <v>5a</v>
-      </c>
-      <c r="AB5" t="str">
+        <v>a</v>
+      </c>
+      <c r="X8" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Y8" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z8" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="AA8" t="str">
         <f t="shared" si="4"/>
         <v>1a</v>
       </c>
-      <c r="AC5" t="str">
+      <c r="AB8" t="str">
         <f t="shared" si="5"/>
-        <v>2b</v>
-      </c>
-      <c r="AD5" t="str">
+        <v>3c</v>
+      </c>
+      <c r="AC8" t="str">
+        <f t="shared" si="6"/>
+        <v>6a</v>
+      </c>
+      <c r="AD8" t="str">
+        <f t="shared" si="7"/>
+        <v>6c</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ8" t="str">
+        <f t="shared" si="8"/>
+        <v>a</v>
+      </c>
+      <c r="AK8" t="str">
+        <f t="shared" si="9"/>
+        <v>h</v>
+      </c>
+      <c r="AL8" t="str">
+        <f t="shared" si="10"/>
+        <v>o</v>
+      </c>
+      <c r="AM8" t="str">
+        <f t="shared" si="11"/>
+        <v>p</v>
+      </c>
+      <c r="AN8" t="str">
+        <f t="shared" si="12"/>
+        <v>ahop</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>15</v>
+      </c>
+      <c r="L9">
+        <v>24</v>
+      </c>
+      <c r="M9">
+        <v>34</v>
+      </c>
+      <c r="N9">
+        <v>60</v>
+      </c>
+      <c r="O9">
+        <v>15</v>
+      </c>
+      <c r="P9">
+        <v>20</v>
+      </c>
+      <c r="Q9">
+        <v>25</v>
+      </c>
+      <c r="R9">
+        <v>35</v>
+      </c>
+      <c r="S9">
+        <v>20</v>
+      </c>
+      <c r="T9">
+        <v>25</v>
+      </c>
+      <c r="U9">
+        <v>35</v>
+      </c>
+      <c r="V9">
+        <v>50</v>
+      </c>
+      <c r="W9" t="str">
+        <f t="shared" si="3"/>
+        <v>c</v>
+      </c>
+      <c r="X9" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y9" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Z9" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="AA9" t="str">
+        <f t="shared" si="4"/>
+        <v>1c</v>
+      </c>
+      <c r="AB9" t="str">
+        <f t="shared" si="5"/>
+        <v>5a</v>
+      </c>
+      <c r="AC9" t="str">
+        <f t="shared" si="6"/>
+        <v>3c</v>
+      </c>
+      <c r="AD9" t="str">
+        <f t="shared" si="7"/>
+        <v>6c</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>42</v>
+      </c>
+      <c r="AJ9" t="str">
+        <f t="shared" si="8"/>
+        <v>c</v>
+      </c>
+      <c r="AK9" t="str">
+        <f t="shared" si="9"/>
+        <v>m</v>
+      </c>
+      <c r="AL9" t="str">
+        <f t="shared" si="10"/>
+        <v>h</v>
+      </c>
+      <c r="AM9" t="str">
+        <f t="shared" si="11"/>
+        <v>p</v>
+      </c>
+      <c r="AN9" t="str">
+        <f t="shared" si="12"/>
+        <v>cmhp</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>5</v>
+      </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10">
+        <v>9</v>
+      </c>
+      <c r="L10">
+        <v>13</v>
+      </c>
+      <c r="M10">
+        <v>18</v>
+      </c>
+      <c r="N10">
+        <v>24</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>65</v>
+      </c>
+      <c r="T10">
+        <v>73</v>
+      </c>
+      <c r="U10">
+        <v>85</v>
+      </c>
+      <c r="V10">
+        <v>99</v>
+      </c>
+      <c r="W10" t="str">
+        <f t="shared" si="3"/>
+        <v>c</v>
+      </c>
+      <c r="X10" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y10" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z10" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA10" t="str">
+        <f t="shared" si="4"/>
+        <v>5c</v>
+      </c>
+      <c r="AB10" t="str">
+        <f t="shared" si="5"/>
+        <v>5a</v>
+      </c>
+      <c r="AC10" t="str">
+        <f t="shared" si="6"/>
+        <v>1a</v>
+      </c>
+      <c r="AD10" t="str">
+        <f t="shared" si="7"/>
+        <v>2a</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AJ10" t="str">
+        <f t="shared" si="8"/>
+        <v>n</v>
+      </c>
+      <c r="AK10" t="str">
+        <f t="shared" si="9"/>
+        <v>m</v>
+      </c>
+      <c r="AL10" t="str">
+        <f t="shared" si="10"/>
+        <v>a</v>
+      </c>
+      <c r="AM10" t="str">
+        <f t="shared" si="11"/>
+        <v>d</v>
+      </c>
+      <c r="AN10" t="str">
+        <f t="shared" si="12"/>
+        <v>nmad</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11">
+        <v>12</v>
+      </c>
+      <c r="L11">
+        <v>20</v>
+      </c>
+      <c r="M11">
+        <v>35</v>
+      </c>
+      <c r="N11">
+        <v>60</v>
+      </c>
+      <c r="O11">
+        <v>22</v>
+      </c>
+      <c r="P11">
+        <v>28</v>
+      </c>
+      <c r="Q11">
+        <v>37</v>
+      </c>
+      <c r="R11">
+        <v>60</v>
+      </c>
+      <c r="S11">
+        <v>35</v>
+      </c>
+      <c r="T11">
+        <v>45</v>
+      </c>
+      <c r="U11">
+        <v>55</v>
+      </c>
+      <c r="V11">
+        <v>75</v>
+      </c>
+      <c r="W11" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X11" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y11" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z11" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA11" t="str">
+        <f t="shared" si="4"/>
+        <v>2a</v>
+      </c>
+      <c r="AB11" t="str">
+        <f t="shared" si="5"/>
+        <v>3a</v>
+      </c>
+      <c r="AC11" t="str">
+        <f t="shared" si="6"/>
+        <v>6a</v>
+      </c>
+      <c r="AD11" t="str">
+        <f t="shared" si="7"/>
+        <v>4a</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ11" t="str">
+        <f t="shared" si="8"/>
+        <v>d</v>
+      </c>
+      <c r="AK11" t="str">
+        <f t="shared" si="9"/>
+        <v>g</v>
+      </c>
+      <c r="AL11" t="str">
+        <f t="shared" si="10"/>
+        <v>o</v>
+      </c>
+      <c r="AM11" t="str">
+        <f t="shared" si="11"/>
+        <v>i</v>
+      </c>
+      <c r="AN11" t="str">
+        <f t="shared" si="12"/>
+        <v>dgoi</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" t="s">
+        <v>10</v>
+      </c>
+      <c r="W12" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X12" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y12" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z12" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA12" t="str">
+        <f t="shared" si="4"/>
+        <v>1a</v>
+      </c>
+      <c r="AB12" t="str">
+        <f t="shared" si="5"/>
+        <v>5a</v>
+      </c>
+      <c r="AC12" t="str">
         <f t="shared" si="6"/>
         <v>3a</v>
       </c>
-      <c r="AF5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG5" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="AD12" t="str">
+        <f t="shared" si="7"/>
+        <v>7a</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>34</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ12" t="str">
+        <f t="shared" si="8"/>
+        <v>a</v>
+      </c>
+      <c r="AK12" t="str">
+        <f t="shared" si="9"/>
+        <v>m</v>
+      </c>
+      <c r="AL12" t="str">
+        <f t="shared" si="10"/>
+        <v>g</v>
+      </c>
+      <c r="AM12" t="str">
+        <f t="shared" si="11"/>
+        <v>q</v>
+      </c>
+      <c r="AN12" t="str">
+        <f t="shared" si="12"/>
+        <v>amgq</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>11</v>
+      </c>
+      <c r="I13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>11</v>
+      </c>
+      <c r="W13" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X13" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Y13" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z13" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="AA13" t="str">
+        <f t="shared" si="4"/>
+        <v>2a</v>
+      </c>
+      <c r="AB13" t="str">
+        <f t="shared" si="5"/>
+        <v>3c</v>
+      </c>
+      <c r="AC13" t="str">
+        <f t="shared" si="6"/>
+        <v>6a</v>
+      </c>
+      <c r="AD13" t="str">
+        <f t="shared" si="7"/>
+        <v>7c</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AI13" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ13" t="str">
+        <f t="shared" si="8"/>
+        <v>d</v>
+      </c>
+      <c r="AK13" t="str">
+        <f t="shared" si="9"/>
+        <v>h</v>
+      </c>
+      <c r="AL13" t="str">
+        <f t="shared" si="10"/>
+        <v>o</v>
+      </c>
+      <c r="AM13" t="str">
+        <f t="shared" si="11"/>
+        <v>r</v>
+      </c>
+      <c r="AN13" t="str">
+        <f t="shared" si="12"/>
+        <v>dhor</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="D14">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" t="s">
+        <v>10</v>
+      </c>
+      <c r="W14" t="str">
+        <f t="shared" si="3"/>
+        <v>c</v>
+      </c>
+      <c r="X14" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y14" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z14" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA14" t="str">
+        <f t="shared" si="4"/>
+        <v>1c</v>
+      </c>
+      <c r="AB14" t="str">
+        <f t="shared" si="5"/>
+        <v>5a</v>
+      </c>
+      <c r="AC14" t="str">
+        <f t="shared" si="6"/>
+        <v>7a</v>
+      </c>
+      <c r="AD14" t="str">
+        <f t="shared" si="7"/>
+        <v>4a</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>39</v>
+      </c>
+      <c r="AI14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ14" t="str">
+        <f t="shared" si="8"/>
+        <v>c</v>
+      </c>
+      <c r="AK14" t="str">
+        <f t="shared" si="9"/>
+        <v>m</v>
+      </c>
+      <c r="AL14" t="str">
+        <f t="shared" si="10"/>
+        <v>q</v>
+      </c>
+      <c r="AM14" t="str">
+        <f t="shared" si="11"/>
+        <v>i</v>
+      </c>
+      <c r="AN14" t="str">
+        <f t="shared" si="12"/>
+        <v>cmqi</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>3</v>
       </c>
-      <c r="F6">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
         <v>3</v>
       </c>
-      <c r="G6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6">
-        <v>15</v>
-      </c>
-      <c r="L6">
-        <v>20</v>
-      </c>
-      <c r="M6">
-        <v>28</v>
-      </c>
-      <c r="N6">
-        <v>33</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>15</v>
-      </c>
-      <c r="R6">
-        <v>20</v>
-      </c>
-      <c r="S6">
-        <v>65</v>
-      </c>
-      <c r="T6">
-        <v>75</v>
-      </c>
-      <c r="U6">
-        <v>40</v>
-      </c>
-      <c r="V6">
-        <v>50</v>
-      </c>
-      <c r="W6" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X6" t="str">
-        <f t="shared" si="0"/>
-        <v>b</v>
-      </c>
-      <c r="Y6" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z6" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="AA6" t="str">
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" t="s">
+        <v>10</v>
+      </c>
+      <c r="W15" t="str">
         <f t="shared" si="3"/>
-        <v>1a</v>
-      </c>
-      <c r="AB6" t="str">
+        <v>a</v>
+      </c>
+      <c r="X15" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y15" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z15" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA15" t="str">
         <f t="shared" si="4"/>
-        <v>2b</v>
-      </c>
-      <c r="AC6" t="str">
+        <v>5a</v>
+      </c>
+      <c r="AB15" t="str">
         <f t="shared" si="5"/>
         <v>3a</v>
       </c>
-      <c r="AD6" t="str">
-        <f t="shared" si="6"/>
-        <v>3c</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7">
-        <v>11</v>
-      </c>
-      <c r="L7">
-        <v>20</v>
-      </c>
-      <c r="M7">
-        <v>25</v>
-      </c>
-      <c r="N7">
-        <v>30</v>
-      </c>
-      <c r="O7">
-        <v>5</v>
-      </c>
-      <c r="P7">
-        <v>7</v>
-      </c>
-      <c r="Q7">
-        <v>12</v>
-      </c>
-      <c r="R7">
-        <v>23</v>
-      </c>
-      <c r="S7">
-        <v>15</v>
-      </c>
-      <c r="T7">
-        <v>23</v>
-      </c>
-      <c r="U7">
-        <v>10</v>
-      </c>
-      <c r="V7">
-        <v>20</v>
-      </c>
-      <c r="W7" t="str">
-        <f t="shared" si="2"/>
-        <v>c</v>
-      </c>
-      <c r="X7" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Y7" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Z7" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA7" t="str">
-        <f t="shared" si="3"/>
-        <v>5c</v>
-      </c>
-      <c r="AB7" t="str">
-        <f t="shared" si="4"/>
-        <v>2c</v>
-      </c>
-      <c r="AC7" t="str">
-        <f t="shared" si="5"/>
-        <v>3c</v>
-      </c>
-      <c r="AD7" t="str">
+      <c r="AC15" t="str">
         <f t="shared" si="6"/>
         <v>6a</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2</v>
-      </c>
-      <c r="B8">
-        <v>2</v>
-      </c>
-      <c r="C8">
+      <c r="AD15" t="str">
+        <f t="shared" si="7"/>
+        <v>8a</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI15" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ15" t="str">
+        <f t="shared" si="8"/>
+        <v>m</v>
+      </c>
+      <c r="AK15" t="str">
+        <f t="shared" si="9"/>
+        <v>g</v>
+      </c>
+      <c r="AL15" t="str">
+        <f t="shared" si="10"/>
+        <v>o</v>
+      </c>
+      <c r="AM15" t="str">
+        <f t="shared" si="11"/>
+        <v>s</v>
+      </c>
+      <c r="AN15" t="str">
+        <f t="shared" si="12"/>
+        <v>mgos</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" t="s">
+        <v>11</v>
+      </c>
+      <c r="W16" t="str">
+        <f t="shared" si="3"/>
+        <v>c</v>
+      </c>
+      <c r="X16" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="Y16" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z16" t="str">
+        <f t="shared" si="0"/>
+        <v>c</v>
+      </c>
+      <c r="AA16" t="str">
+        <f t="shared" si="4"/>
+        <v>5c</v>
+      </c>
+      <c r="AB16" t="str">
+        <f t="shared" si="5"/>
+        <v>7c</v>
+      </c>
+      <c r="AC16" t="str">
+        <f t="shared" si="6"/>
+        <v>8a</v>
+      </c>
+      <c r="AD16" t="str">
+        <f t="shared" si="7"/>
+        <v>4c</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>49</v>
+      </c>
+      <c r="AI16" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ16" t="str">
+        <f t="shared" si="8"/>
+        <v>n</v>
+      </c>
+      <c r="AK16" t="str">
+        <f t="shared" si="9"/>
+        <v>r</v>
+      </c>
+      <c r="AL16" t="str">
+        <f t="shared" si="10"/>
+        <v>s</v>
+      </c>
+      <c r="AM16" t="str">
+        <f t="shared" si="11"/>
+        <v>j</v>
+      </c>
+      <c r="AN16" t="str">
+        <f t="shared" si="12"/>
+        <v>nrsj</v>
+      </c>
+    </row>
+    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>1</v>
       </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-      <c r="E8">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>8</v>
+      </c>
+      <c r="G17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+      <c r="I17" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" t="s">
+        <v>10</v>
+      </c>
+      <c r="W17" t="str">
+        <f t="shared" si="3"/>
+        <v>b</v>
+      </c>
+      <c r="X17" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Y17" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="Z17" t="str">
+        <f t="shared" si="0"/>
+        <v>a</v>
+      </c>
+      <c r="AA17" t="str">
+        <f t="shared" si="4"/>
+        <v>1b</v>
+      </c>
+      <c r="AB17" t="str">
+        <f t="shared" si="5"/>
+        <v>5a</v>
+      </c>
+      <c r="AC17" t="str">
+        <f t="shared" si="6"/>
+        <v>7a</v>
+      </c>
+      <c r="AD17" t="str">
+        <f t="shared" si="7"/>
+        <v>8a</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>71</v>
+      </c>
+      <c r="AJ17" t="str">
+        <f t="shared" si="8"/>
+        <v>b</v>
+      </c>
+      <c r="AK17" t="str">
+        <f t="shared" si="9"/>
+        <v>m</v>
+      </c>
+      <c r="AL17" t="str">
+        <f t="shared" si="10"/>
+        <v>q</v>
+      </c>
+      <c r="AM17" t="str">
+        <f t="shared" si="11"/>
+        <v>s</v>
+      </c>
+      <c r="AN17" t="str">
+        <f t="shared" si="12"/>
+        <v>bmqs</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
         <v>6</v>
       </c>
-      <c r="F8">
-        <v>6</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8">
-        <v>12</v>
-      </c>
-      <c r="L8">
-        <v>15</v>
-      </c>
-      <c r="M8">
-        <v>30</v>
-      </c>
-      <c r="N8">
-        <v>50</v>
-      </c>
-      <c r="O8">
-        <v>11</v>
-      </c>
-      <c r="P8">
-        <v>16</v>
-      </c>
-      <c r="Q8">
-        <v>22</v>
-      </c>
-      <c r="R8">
-        <v>30</v>
-      </c>
-      <c r="S8">
-        <v>15</v>
-      </c>
-      <c r="T8">
-        <v>20</v>
-      </c>
-      <c r="U8">
-        <v>25</v>
-      </c>
-      <c r="V8">
-        <v>45</v>
-      </c>
-      <c r="W8" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X8" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Y8" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z8" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="AA8" t="str">
+      <c r="E18">
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" t="s">
+        <v>40</v>
+      </c>
+      <c r="W18" t="str">
         <f t="shared" si="3"/>
-        <v>1a</v>
-      </c>
-      <c r="AB8" t="str">
+        <v>a</v>
+      </c>
+      <c r="X18" t="str">
+        <f t="shared" ref="X18:X21" si="13">VLOOKUP(H18,$AF$2:$AG$6,2,FALSE)</f>
+        <v>a</v>
+      </c>
+      <c r="Y18" t="str">
+        <f t="shared" ref="Y18:Y21" si="14">VLOOKUP(I18,$AF$2:$AG$6,2,FALSE)</f>
+        <v>a</v>
+      </c>
+      <c r="Z18" t="str">
+        <f t="shared" ref="Z18:Z21" si="15">VLOOKUP(J18,$AF$2:$AG$6,2,FALSE)</f>
+        <v>d</v>
+      </c>
+      <c r="AA18" t="str">
         <f t="shared" si="4"/>
-        <v>3c</v>
-      </c>
-      <c r="AC8" t="str">
+        <v>2a</v>
+      </c>
+      <c r="AB18" t="str">
         <f t="shared" si="5"/>
         <v>6a</v>
       </c>
-      <c r="AD8" t="str">
+      <c r="AC18" t="str">
         <f t="shared" si="6"/>
-        <v>6c</v>
-      </c>
-    </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
+        <v>8a</v>
+      </c>
+      <c r="AD18" t="str">
+        <f t="shared" si="7"/>
+        <v>4d</v>
+      </c>
+      <c r="AH18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AI18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ18" t="str">
+        <f t="shared" si="8"/>
+        <v>d</v>
+      </c>
+      <c r="AK18" t="str">
+        <f t="shared" si="9"/>
+        <v>o</v>
+      </c>
+      <c r="AL18" t="str">
+        <f t="shared" si="10"/>
+        <v>s</v>
+      </c>
+      <c r="AM18" t="str">
+        <f t="shared" si="11"/>
+        <v>k</v>
+      </c>
+      <c r="AN18" t="str">
+        <f t="shared" si="12"/>
+        <v>dosk</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
+      <c r="C19">
         <v>5</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="D19">
+        <v>7</v>
+      </c>
+      <c r="E19">
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
         <v>11</v>
       </c>
-      <c r="H9" t="s">
-        <v>10</v>
-      </c>
-      <c r="I9" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9">
-        <v>15</v>
-      </c>
-      <c r="L9">
-        <v>24</v>
-      </c>
-      <c r="M9">
-        <v>34</v>
-      </c>
-      <c r="N9">
-        <v>60</v>
-      </c>
-      <c r="O9">
-        <v>15</v>
-      </c>
-      <c r="P9">
-        <v>20</v>
-      </c>
-      <c r="Q9">
-        <v>25</v>
-      </c>
-      <c r="R9">
-        <v>35</v>
-      </c>
-      <c r="S9">
-        <v>20</v>
-      </c>
-      <c r="T9">
-        <v>25</v>
-      </c>
-      <c r="U9">
-        <v>35</v>
-      </c>
-      <c r="V9">
-        <v>50</v>
-      </c>
-      <c r="W9" t="str">
-        <f t="shared" si="2"/>
+      <c r="I19" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" t="s">
+        <v>41</v>
+      </c>
+      <c r="W19" t="str">
+        <f t="shared" si="3"/>
+        <v>a</v>
+      </c>
+      <c r="X19" t="str">
+        <f t="shared" si="13"/>
         <v>c</v>
       </c>
-      <c r="X9" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y9" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Z9" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="AA9" t="str">
-        <f t="shared" si="3"/>
-        <v>1c</v>
-      </c>
-      <c r="AB9" t="str">
+      <c r="Y19" t="str">
+        <f t="shared" si="14"/>
+        <v>a</v>
+      </c>
+      <c r="Z19" t="str">
+        <f t="shared" si="15"/>
+        <v>e</v>
+      </c>
+      <c r="AA19" t="str">
         <f t="shared" si="4"/>
         <v>5a</v>
       </c>
-      <c r="AC9" t="str">
+      <c r="AB19" t="str">
         <f t="shared" si="5"/>
-        <v>3c</v>
-      </c>
-      <c r="AD9" t="str">
+        <v>7c</v>
+      </c>
+      <c r="AC19" t="str">
         <f t="shared" si="6"/>
-        <v>6c</v>
-      </c>
-    </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>4</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
-      </c>
-      <c r="D10">
-        <v>5</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" t="s">
-        <v>10</v>
-      </c>
-      <c r="J10" t="s">
-        <v>10</v>
-      </c>
-      <c r="K10">
-        <v>9</v>
-      </c>
-      <c r="L10">
-        <v>13</v>
-      </c>
-      <c r="M10">
-        <v>18</v>
-      </c>
-      <c r="N10">
-        <v>24</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>65</v>
-      </c>
-      <c r="T10">
+        <v>8a</v>
+      </c>
+      <c r="AD19" t="str">
+        <f t="shared" si="7"/>
+        <v>4e</v>
+      </c>
+      <c r="AH19" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI19" t="s">
         <v>73</v>
       </c>
-      <c r="U10">
-        <v>85</v>
-      </c>
-      <c r="V10">
-        <v>99</v>
-      </c>
-      <c r="W10" t="str">
-        <f t="shared" si="2"/>
-        <v>c</v>
-      </c>
-      <c r="X10" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y10" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z10" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA10" t="str">
+      <c r="AJ19" t="str">
+        <f t="shared" si="8"/>
+        <v>m</v>
+      </c>
+      <c r="AK19" t="str">
+        <f t="shared" si="9"/>
+        <v>r</v>
+      </c>
+      <c r="AL19" t="str">
+        <f t="shared" si="10"/>
+        <v>s</v>
+      </c>
+      <c r="AM19" t="str">
+        <f t="shared" si="11"/>
+        <v>l</v>
+      </c>
+      <c r="AN19" t="str">
+        <f t="shared" si="12"/>
+        <v>mrsl</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>7</v>
+      </c>
+      <c r="F20">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" t="s">
+        <v>10</v>
+      </c>
+      <c r="W20" t="str">
         <f t="shared" si="3"/>
-        <v>5c</v>
-      </c>
-      <c r="AB10" t="str">
-        <f t="shared" si="4"/>
-        <v>5a</v>
-      </c>
-      <c r="AC10" t="str">
-        <f t="shared" si="5"/>
-        <v>1a</v>
-      </c>
-      <c r="AD10" t="str">
-        <f t="shared" si="6"/>
-        <v>2a</v>
-      </c>
-    </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>6</v>
-      </c>
-      <c r="F11">
-        <v>4</v>
-      </c>
-      <c r="G11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11">
-        <v>12</v>
-      </c>
-      <c r="L11">
-        <v>20</v>
-      </c>
-      <c r="M11">
-        <v>35</v>
-      </c>
-      <c r="N11">
-        <v>60</v>
-      </c>
-      <c r="O11">
-        <v>22</v>
-      </c>
-      <c r="P11">
-        <v>28</v>
-      </c>
-      <c r="Q11">
-        <v>37</v>
-      </c>
-      <c r="R11">
-        <v>60</v>
-      </c>
-      <c r="S11">
-        <v>35</v>
-      </c>
-      <c r="T11">
-        <v>45</v>
-      </c>
-      <c r="U11">
-        <v>55</v>
-      </c>
-      <c r="V11">
-        <v>75</v>
-      </c>
-      <c r="W11" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X11" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y11" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z11" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA11" t="str">
-        <f t="shared" si="3"/>
-        <v>2a</v>
-      </c>
-      <c r="AB11" t="str">
+        <v>a</v>
+      </c>
+      <c r="X20" t="str">
+        <f t="shared" si="13"/>
+        <v>a</v>
+      </c>
+      <c r="Y20" t="str">
+        <f t="shared" si="14"/>
+        <v>a</v>
+      </c>
+      <c r="Z20" t="str">
+        <f t="shared" si="15"/>
+        <v>a</v>
+      </c>
+      <c r="AA20" t="str">
         <f t="shared" si="4"/>
         <v>3a</v>
       </c>
-      <c r="AC11" t="str">
+      <c r="AB20" t="str">
         <f t="shared" si="5"/>
         <v>6a</v>
       </c>
-      <c r="AD11" t="str">
-        <f t="shared" si="6"/>
-        <v>4a</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
-      </c>
-      <c r="H12" t="s">
-        <v>10</v>
-      </c>
-      <c r="I12" t="s">
-        <v>10</v>
-      </c>
-      <c r="J12" t="s">
-        <v>10</v>
-      </c>
-      <c r="W12" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X12" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y12" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z12" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA12" t="str">
-        <f t="shared" si="3"/>
-        <v>1a</v>
-      </c>
-      <c r="AB12" t="str">
-        <f t="shared" si="4"/>
-        <v>5a</v>
-      </c>
-      <c r="AC12" t="str">
-        <f t="shared" si="5"/>
-        <v>3a</v>
-      </c>
-      <c r="AD12" t="str">
+      <c r="AC20" t="str">
         <f t="shared" si="6"/>
         <v>7a</v>
       </c>
-    </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>6</v>
-      </c>
-      <c r="F13">
-        <v>7</v>
-      </c>
-      <c r="G13" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" t="s">
-        <v>11</v>
-      </c>
-      <c r="W13" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X13" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Y13" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z13" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="AA13" t="str">
-        <f t="shared" si="3"/>
-        <v>2a</v>
-      </c>
-      <c r="AB13" t="str">
+      <c r="AD20" t="str">
+        <f t="shared" si="7"/>
+        <v>8a</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ20" t="str">
+        <f t="shared" si="8"/>
+        <v>g</v>
+      </c>
+      <c r="AK20" t="str">
+        <f t="shared" si="9"/>
+        <v>o</v>
+      </c>
+      <c r="AL20" t="str">
+        <f t="shared" si="10"/>
+        <v>q</v>
+      </c>
+      <c r="AM20" t="str">
+        <f t="shared" si="11"/>
+        <v>s</v>
+      </c>
+      <c r="AN20" t="str">
+        <f t="shared" si="12"/>
+        <v>goqs</v>
+      </c>
+    </row>
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="F21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J21" t="s">
+        <v>41</v>
+      </c>
+      <c r="W21" t="str">
+        <f>VLOOKUP(G21,$AF$2:$AG$6,2,FALSE)</f>
+        <v>a</v>
+      </c>
+      <c r="X21" t="str">
+        <f t="shared" si="13"/>
+        <v>a</v>
+      </c>
+      <c r="Y21" t="str">
+        <f t="shared" si="14"/>
+        <v>d</v>
+      </c>
+      <c r="Z21" t="str">
+        <f t="shared" si="15"/>
+        <v>e</v>
+      </c>
+      <c r="AA21" t="str">
         <f t="shared" si="4"/>
-        <v>3c</v>
-      </c>
-      <c r="AC13" t="str">
+        <v>1a</v>
+      </c>
+      <c r="AB21" t="str">
         <f t="shared" si="5"/>
-        <v>6a</v>
-      </c>
-      <c r="AD13" t="str">
-        <f t="shared" si="6"/>
-        <v>7c</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>3</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>5</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="F14">
-        <v>4</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>10</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
-      </c>
-      <c r="J14" t="s">
-        <v>10</v>
-      </c>
-      <c r="W14" t="str">
-        <f t="shared" si="2"/>
-        <v>c</v>
-      </c>
-      <c r="X14" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y14" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z14" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA14" t="str">
-        <f t="shared" si="3"/>
-        <v>1c</v>
-      </c>
-      <c r="AB14" t="str">
-        <f t="shared" si="4"/>
-        <v>5a</v>
-      </c>
-      <c r="AC14" t="str">
-        <f t="shared" si="5"/>
-        <v>7a</v>
-      </c>
-      <c r="AD14" t="str">
-        <f t="shared" si="6"/>
         <v>4a</v>
       </c>
-    </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>3</v>
-      </c>
-      <c r="B15">
-        <v>4</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15">
-        <v>6</v>
-      </c>
-      <c r="F15">
-        <v>8</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" t="s">
-        <v>10</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J15" t="s">
-        <v>10</v>
-      </c>
-      <c r="W15" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X15" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y15" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z15" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA15" t="str">
-        <f t="shared" si="3"/>
-        <v>5a</v>
-      </c>
-      <c r="AB15" t="str">
-        <f t="shared" si="4"/>
-        <v>3a</v>
-      </c>
-      <c r="AC15" t="str">
-        <f t="shared" si="5"/>
-        <v>6a</v>
-      </c>
-      <c r="AD15" t="str">
-        <f t="shared" si="6"/>
-        <v>8a</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>3</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-      <c r="E16">
-        <v>8</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>11</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
-      </c>
-      <c r="J16" t="s">
-        <v>11</v>
-      </c>
-      <c r="W16" t="str">
-        <f t="shared" si="2"/>
-        <v>c</v>
-      </c>
-      <c r="X16" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="Y16" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z16" t="str">
-        <f t="shared" si="0"/>
-        <v>c</v>
-      </c>
-      <c r="AA16" t="str">
-        <f t="shared" si="3"/>
-        <v>5c</v>
-      </c>
-      <c r="AB16" t="str">
-        <f t="shared" si="4"/>
-        <v>7c</v>
-      </c>
-      <c r="AC16" t="str">
-        <f t="shared" si="5"/>
-        <v>8a</v>
-      </c>
-      <c r="AD16" t="str">
-        <f t="shared" si="6"/>
-        <v>4c</v>
-      </c>
-    </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>4</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="F17">
-        <v>8</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" t="s">
-        <v>10</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
-      </c>
-      <c r="J17" t="s">
-        <v>10</v>
-      </c>
-      <c r="W17" t="str">
-        <f t="shared" si="2"/>
-        <v>b</v>
-      </c>
-      <c r="X17" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Y17" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="Z17" t="str">
-        <f t="shared" si="0"/>
-        <v>a</v>
-      </c>
-      <c r="AA17" t="str">
-        <f t="shared" si="3"/>
-        <v>1b</v>
-      </c>
-      <c r="AB17" t="str">
-        <f t="shared" si="4"/>
-        <v>5a</v>
-      </c>
-      <c r="AC17" t="str">
-        <f t="shared" si="5"/>
-        <v>7a</v>
-      </c>
-      <c r="AD17" t="str">
-        <f t="shared" si="6"/>
-        <v>8a</v>
-      </c>
-    </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>4</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>8</v>
-      </c>
-      <c r="F18">
-        <v>4</v>
-      </c>
-      <c r="G18" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" t="s">
-        <v>40</v>
-      </c>
-      <c r="W18" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X18" t="str">
-        <f t="shared" ref="X18:X21" si="7">VLOOKUP(H18,$AF$2:$AG$6,2,FALSE)</f>
-        <v>a</v>
-      </c>
-      <c r="Y18" t="str">
-        <f t="shared" ref="Y18:Y21" si="8">VLOOKUP(I18,$AF$2:$AG$6,2,FALSE)</f>
-        <v>a</v>
-      </c>
-      <c r="Z18" t="str">
-        <f t="shared" ref="Z18:Z21" si="9">VLOOKUP(J18,$AF$2:$AG$6,2,FALSE)</f>
-        <v>d</v>
-      </c>
-      <c r="AA18" t="str">
-        <f t="shared" si="3"/>
-        <v>2a</v>
-      </c>
-      <c r="AB18" t="str">
-        <f t="shared" si="4"/>
-        <v>6a</v>
-      </c>
-      <c r="AC18" t="str">
-        <f t="shared" si="5"/>
-        <v>8a</v>
-      </c>
-      <c r="AD18" t="str">
+      <c r="AC21" t="str">
         <f t="shared" si="6"/>
         <v>4d</v>
       </c>
-    </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>4</v>
-      </c>
-      <c r="B19">
-        <v>3</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19">
-        <v>8</v>
-      </c>
-      <c r="F19">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
-      </c>
-      <c r="J19" t="s">
-        <v>41</v>
-      </c>
-      <c r="W19" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X19" t="str">
+      <c r="AD21" t="str">
         <f t="shared" si="7"/>
-        <v>c</v>
-      </c>
-      <c r="Y19" t="str">
+        <v>4e</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ21" t="str">
         <f t="shared" si="8"/>
         <v>a</v>
       </c>
-      <c r="Z19" t="str">
+      <c r="AK21" t="str">
         <f t="shared" si="9"/>
-        <v>e</v>
-      </c>
-      <c r="AA19" t="str">
-        <f t="shared" si="3"/>
-        <v>5a</v>
-      </c>
-      <c r="AB19" t="str">
-        <f t="shared" si="4"/>
-        <v>7c</v>
-      </c>
-      <c r="AC19" t="str">
-        <f t="shared" si="5"/>
-        <v>8a</v>
-      </c>
-      <c r="AD19" t="str">
-        <f t="shared" si="6"/>
-        <v>4e</v>
-      </c>
-    </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="B20">
-        <v>4</v>
-      </c>
-      <c r="C20">
-        <v>3</v>
-      </c>
-      <c r="D20">
-        <v>6</v>
-      </c>
-      <c r="E20">
-        <v>7</v>
-      </c>
-      <c r="F20">
-        <v>8</v>
-      </c>
-      <c r="G20" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" t="s">
-        <v>10</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
-      </c>
-      <c r="W20" t="str">
-        <f t="shared" si="2"/>
-        <v>a</v>
-      </c>
-      <c r="X20" t="str">
-        <f t="shared" si="7"/>
-        <v>a</v>
-      </c>
-      <c r="Y20" t="str">
-        <f t="shared" si="8"/>
-        <v>a</v>
-      </c>
-      <c r="Z20" t="str">
-        <f t="shared" si="9"/>
-        <v>a</v>
-      </c>
-      <c r="AA20" t="str">
-        <f t="shared" si="3"/>
-        <v>3a</v>
-      </c>
-      <c r="AB20" t="str">
-        <f t="shared" si="4"/>
-        <v>6a</v>
-      </c>
-      <c r="AC20" t="str">
-        <f t="shared" si="5"/>
-        <v>7a</v>
-      </c>
-      <c r="AD20" t="str">
-        <f t="shared" si="6"/>
-        <v>8a</v>
-      </c>
-    </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>4</v>
-      </c>
-      <c r="B21">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21">
-        <v>4</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="F21">
-        <v>4</v>
-      </c>
-      <c r="G21" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" t="s">
-        <v>10</v>
-      </c>
-      <c r="I21" t="s">
-        <v>40</v>
-      </c>
-      <c r="J21" t="s">
-        <v>41</v>
-      </c>
-      <c r="W21" t="str">
-        <f>VLOOKUP(G21,$AF$2:$AG$6,2,FALSE)</f>
-        <v>a</v>
-      </c>
-      <c r="X21" t="str">
-        <f t="shared" si="7"/>
-        <v>a</v>
-      </c>
-      <c r="Y21" t="str">
-        <f t="shared" si="8"/>
-        <v>d</v>
-      </c>
-      <c r="Z21" t="str">
-        <f t="shared" si="9"/>
-        <v>e</v>
-      </c>
-      <c r="AA21" t="str">
-        <f t="shared" si="3"/>
-        <v>1a</v>
-      </c>
-      <c r="AB21" t="str">
-        <f t="shared" si="4"/>
-        <v>4a</v>
-      </c>
-      <c r="AC21" t="str">
-        <f t="shared" si="5"/>
-        <v>4d</v>
-      </c>
-      <c r="AD21" t="str">
-        <f t="shared" si="6"/>
-        <v>4e</v>
+        <v>i</v>
+      </c>
+      <c r="AL21" t="str">
+        <f t="shared" si="10"/>
+        <v>k</v>
+      </c>
+      <c r="AM21" t="str">
+        <f t="shared" si="11"/>
+        <v>l</v>
+      </c>
+      <c r="AN21" t="str">
+        <f t="shared" si="12"/>
+        <v>aikl</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AH22" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AH23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI23" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AH24" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI24" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2316,11 +2903,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T80"/>
+  <dimension ref="A1:V80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2335,7 +2920,7 @@
     <col min="19" max="19" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>28</v>
       </c>
@@ -2382,7 +2967,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -2429,7 +3014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -2476,7 +3061,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -2523,7 +3108,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2570,7 +3155,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2617,7 +3202,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -2664,7 +3249,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2711,7 +3296,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -2751,8 +3336,16 @@
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="T9">
+        <f>SUM(T1:T8)</f>
+        <v>19</v>
+      </c>
+      <c r="V9">
+        <f>T9*14</f>
+        <v>266</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -2799,7 +3392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -2840,7 +3433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -2881,7 +3474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -2922,7 +3515,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -2963,7 +3556,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -3004,7 +3597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>48</v>
       </c>

</xml_diff>

<commit_message>
new sprites used... todo: fix new vsynccount issue
git-svn-id: https://svn.code.sf.net/p/castle-defender/code/trunk@47 44b1cee5-f01f-473f-a638-7a13f5ae6cd1
</commit_message>
<xml_diff>
--- a/waves/waves and enemies.xlsx
+++ b/waves/waves and enemies.xlsx
@@ -589,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="AH4" workbookViewId="0">
+      <selection activeCell="AK15" sqref="AK15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1194,7 +1194,7 @@
         <v>g</v>
       </c>
       <c r="AN5" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ5,AK5,AL5,AM5)</f>
         <v>maeg</v>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
         <v>h</v>
       </c>
       <c r="AN6" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ6,AK6,AL6,AM6)</f>
         <v>aegh</v>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
         <v>q</v>
       </c>
       <c r="AN12" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ12,AK12,AL12,AM12)</f>
         <v>amgq</v>
       </c>
     </row>
@@ -2496,7 +2496,7 @@
         <v>s</v>
       </c>
       <c r="AN17" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ17,AK17,AL17,AM17)</f>
         <v>bmqs</v>
       </c>
     </row>
@@ -2586,7 +2586,7 @@
         <v>k</v>
       </c>
       <c r="AN18" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ18,AK18,AL18,AM18)</f>
         <v>dosk</v>
       </c>
     </row>
@@ -2676,7 +2676,7 @@
         <v>l</v>
       </c>
       <c r="AN19" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ19,AK19,AL19,AM19)</f>
         <v>mrsl</v>
       </c>
     </row>
@@ -2766,7 +2766,7 @@
         <v>s</v>
       </c>
       <c r="AN20" t="str">
-        <f t="shared" si="12"/>
+        <f>CONCATENATE(AJ20,AK20,AL20,AM20)</f>
         <v>goqs</v>
       </c>
     </row>

</xml_diff>